<commit_message>
civil and ece dept change
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/004.xlsx
+++ b/docs/STAFF-DATA/004.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E128E40-EAF1-41FA-B5AC-F607C30F1ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15036" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -118,18 +117,6 @@
     <t>VEC-004-04-066</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/004/VEC-004-04-070.webp</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?hl=en&amp;view_op=list_works&amp;gmla=ALUCkoWRiJG96gXC-1I4xAEBjfrAGcOjmEE5O8YwipOj-GDcbpKpLcK4qYn97vSs8zU-</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/gopinath-selvaraj-7510a7120/</t>
-  </si>
-  <si>
-    <t>VEC-004-04-070</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/004/VEC-004-04-061.webp</t>
   </si>
   <si>
@@ -145,18 +132,6 @@
     <t>VEC-004-04-061</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/004/VEC-004-04-073.webp</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?view_op=list_works&amp;hl=en&amp;user=faR6u3kAAAAJ&amp;gmla=ALUCkoVkPAxOsBHpg4cCVzWObCOEQ5hbm_o9JoKjBSED0ga-bsdtimOOkRubIe0o8Jde8vG3Mfhnff50Co6jgAk76RN5ECufXoFHkk_KfPDCDgMQWg</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/me?trk=p_mwlite_profile_view-secondary_nav</t>
-  </si>
-  <si>
-    <t>VEC-004-04-073</t>
-  </si>
-  <si>
     <t>Dr. JEBAMALAR A</t>
   </si>
   <si>
@@ -166,13 +141,7 @@
     <t>Mr. RAJHARASEHWARAN T A</t>
   </si>
   <si>
-    <t>Mr. GOPINATH S</t>
-  </si>
-  <si>
     <t>Mr. RAJENDHIRAN K</t>
-  </si>
-  <si>
-    <t>Mr. RAJASEKAR G</t>
   </si>
   <si>
     <t>VEC-004-04-601</t>
@@ -205,7 +174,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,14 +549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,7 +607,7 @@
     </row>
     <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -670,7 +639,7 @@
     </row>
     <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -696,7 +665,7 @@
     </row>
     <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -717,9 +686,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -727,101 +696,65 @@
       <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>33</v>
       </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" t="s">
         <v>42</v>
-      </c>
-      <c r="I7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" t="s">
-        <v>53</v>
-      </c>
-    </row>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
     </row>

</xml_diff>